<commit_message>
add complexity to excel sample
</commit_message>
<xml_diff>
--- a/data/villa_fc.xlsx
+++ b/data/villa_fc.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t xml:space="preserve">NOMBRE</t>
   </si>
@@ -40,31 +40,34 @@
     <t xml:space="preserve">Gil</t>
   </si>
   <si>
+    <t xml:space="preserve">2023/12/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebasti4n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cortes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/07/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/04/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacobo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montenegro</t>
+  </si>
+  <si>
     <t xml:space="preserve">28/12/2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebasti4n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cortes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14/07/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manuela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Correa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15/04/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jacobo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montenegro</t>
   </si>
   <si>
     <t xml:space="preserve">Daniel</t>
@@ -106,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -194,10 +198,10 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.14"/>
   </cols>
@@ -269,74 +273,74 @@
         <v>3233073789</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>3235837848</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>3193917279</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>28304</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>3165326067</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>3157266898</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>